<commit_message>
added soils and updated SM data
</commit_message>
<xml_diff>
--- a/Data/SM/NutNet_SM_051118.xlsx
+++ b/Data/SM/NutNet_SM_051118.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicksmith/Documents/Research/NutNet/Data/SM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{583D52F0-F8CE-624A-A4FE-741322B2DF68}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{61D16613-58CC-D440-96EF-2841DD97E5EE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8960" yWindow="1220" windowWidth="28040" windowHeight="17440" xr2:uid="{CB6837DA-25D4-4A48-8034-FE21B8DC23E0}"/>
   </bookViews>
@@ -384,8 +384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8E8B63F-C54E-7F44-869C-0FB4DB559B4C}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>